<commit_message>
corrected w2.py in Workshop 2.11
</commit_message>
<xml_diff>
--- a/Agenda - CE-QUAL-W2_Workshop_Aug_2022.xlsx
+++ b/Agenda - CE-QUAL-W2_Workshop_Aug_2022.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/todd/GitHub/environmentalsystems/CE-QUAL-W2/workshop/2022/Agenda/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/todd/GitHub/environmentalsystems/CE-QUAL-W2-Workshop-2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C9C2FE-2AA8-7D49-AD8B-0ACE5484694F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FAAECE-8F3A-F545-A5D6-53B3AD82073B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{5524DC16-E37C-514A-B687-063004997C4D}"/>
   </bookViews>
@@ -790,52 +790,22 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -901,6 +871,24 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -910,10 +898,22 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1242,8 +1242,8 @@
   </sheetPr>
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33:E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1261,36 +1261,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
     </row>
     <row r="3" spans="1:9" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="97"/>
+      <c r="B3" s="59"/>
       <c r="C3" s="33"/>
-      <c r="D3" s="97" t="s">
+      <c r="D3" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97" t="s">
+      <c r="E3" s="59"/>
+      <c r="F3" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97" t="s">
+      <c r="G3" s="59"/>
+      <c r="H3" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="97"/>
+      <c r="I3" s="59"/>
     </row>
     <row r="4" spans="1:9" s="24" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -1390,10 +1390,10 @@
       <c r="B8" s="2">
         <v>0.39583333333333298</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="D8" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="59"/>
+      <c r="E8" s="61"/>
       <c r="F8" s="43"/>
       <c r="G8" s="29"/>
       <c r="H8" s="51"/>
@@ -1406,16 +1406,16 @@
       <c r="B9" s="2">
         <v>0.40625</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="56" t="s">
+      <c r="D9" s="62"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="57"/>
-      <c r="H9" s="56" t="s">
+      <c r="G9" s="58"/>
+      <c r="H9" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="I9" s="57"/>
+      <c r="I9" s="58"/>
     </row>
     <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
@@ -1512,18 +1512,18 @@
       <c r="B14" s="2">
         <v>0.45833333333333298</v>
       </c>
-      <c r="D14" s="56" t="s">
+      <c r="D14" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="57"/>
-      <c r="F14" s="56" t="s">
+      <c r="E14" s="58"/>
+      <c r="F14" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="57"/>
-      <c r="H14" s="56" t="s">
+      <c r="G14" s="58"/>
+      <c r="H14" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="I14" s="57"/>
+      <c r="I14" s="58"/>
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
@@ -1620,18 +1620,18 @@
       <c r="B19" s="2">
         <v>0.51041666666666696</v>
       </c>
-      <c r="D19" s="66" t="s">
+      <c r="D19" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="67"/>
-      <c r="F19" s="60" t="s">
+      <c r="E19" s="93"/>
+      <c r="F19" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="61"/>
-      <c r="H19" s="60" t="s">
+      <c r="G19" s="84"/>
+      <c r="H19" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="61"/>
+      <c r="I19" s="84"/>
     </row>
     <row r="20" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
@@ -1640,12 +1640,12 @@
       <c r="B20" s="2">
         <v>0.52083333333333304</v>
       </c>
-      <c r="D20" s="68"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="63"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="95"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="86"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="86"/>
     </row>
     <row r="21" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
@@ -1654,12 +1654,12 @@
       <c r="B21" s="2">
         <v>0.53125</v>
       </c>
-      <c r="D21" s="68"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="63"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="63"/>
+      <c r="D21" s="94"/>
+      <c r="E21" s="95"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="86"/>
+      <c r="H21" s="85"/>
+      <c r="I21" s="86"/>
     </row>
     <row r="22" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
@@ -1668,12 +1668,12 @@
       <c r="B22" s="2">
         <v>0.54166666666666696</v>
       </c>
-      <c r="D22" s="68"/>
-      <c r="E22" s="69"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="63"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="63"/>
+      <c r="D22" s="94"/>
+      <c r="E22" s="95"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="86"/>
+      <c r="H22" s="85"/>
+      <c r="I22" s="86"/>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
@@ -1682,12 +1682,12 @@
       <c r="B23" s="2">
         <v>0.55208333333333304</v>
       </c>
-      <c r="D23" s="68"/>
-      <c r="E23" s="69"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="63"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="63"/>
+      <c r="D23" s="94"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="86"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="86"/>
     </row>
     <row r="24" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
@@ -1696,12 +1696,12 @@
       <c r="B24" s="2">
         <v>0.5625</v>
       </c>
-      <c r="D24" s="70"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="64"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="64"/>
-      <c r="I24" s="65"/>
+      <c r="D24" s="96"/>
+      <c r="E24" s="97"/>
+      <c r="F24" s="87"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="87"/>
+      <c r="I24" s="88"/>
     </row>
     <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
@@ -1776,10 +1776,10 @@
       <c r="B28" s="2">
         <v>0.60416666666666696</v>
       </c>
-      <c r="D28" s="56" t="s">
+      <c r="D28" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="57"/>
+      <c r="E28" s="58"/>
       <c r="F28" s="12"/>
       <c r="G28" s="15"/>
       <c r="H28" s="45"/>
@@ -1798,10 +1798,10 @@
       <c r="E29" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F29" s="56" t="s">
+      <c r="F29" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="G29" s="57"/>
+      <c r="G29" s="58"/>
       <c r="H29" s="45"/>
       <c r="I29" s="14"/>
     </row>
@@ -1838,10 +1838,10 @@
       </c>
       <c r="F31" s="46"/>
       <c r="G31" s="29"/>
-      <c r="H31" s="58" t="s">
+      <c r="H31" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="I31" s="59"/>
+      <c r="I31" s="61"/>
     </row>
     <row r="32" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
@@ -1872,10 +1872,10 @@
       <c r="B33" s="2">
         <v>0.65625</v>
       </c>
-      <c r="D33" s="56" t="s">
+      <c r="D33" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E33" s="57"/>
+      <c r="E33" s="58"/>
       <c r="F33" s="12"/>
       <c r="G33" s="47"/>
       <c r="H33" s="55"/>
@@ -1894,10 +1894,10 @@
       <c r="E34" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F34" s="56" t="s">
+      <c r="F34" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="G34" s="95"/>
+      <c r="G34" s="91"/>
       <c r="H34" s="31"/>
       <c r="I34" s="20"/>
     </row>
@@ -1919,7 +1919,7 @@
       <c r="H35" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="I35" s="48" t="s">
+      <c r="I35" s="18" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1949,94 +1949,78 @@
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="7"/>
-      <c r="H38" s="76" t="s">
+      <c r="H38" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="I38" s="76"/>
+      <c r="I38" s="66"/>
     </row>
     <row r="39" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="8"/>
-      <c r="D39" s="77" t="s">
+      <c r="D39" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="E39" s="78"/>
+      <c r="E39" s="68"/>
       <c r="F39" s="33"/>
-      <c r="H39" s="83" t="s">
+      <c r="H39" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="I39" s="84"/>
+      <c r="I39" s="74"/>
     </row>
     <row r="40" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
-      <c r="D40" s="79"/>
-      <c r="E40" s="80"/>
-      <c r="H40" s="85" t="s">
+      <c r="D40" s="69"/>
+      <c r="E40" s="70"/>
+      <c r="H40" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="I40" s="86"/>
+      <c r="I40" s="76"/>
     </row>
     <row r="41" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
-      <c r="D41" s="79"/>
-      <c r="E41" s="80"/>
-      <c r="H41" s="87" t="s">
+      <c r="D41" s="69"/>
+      <c r="E41" s="70"/>
+      <c r="H41" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="I41" s="88"/>
+      <c r="I41" s="78"/>
     </row>
     <row r="42" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
-      <c r="D42" s="79"/>
-      <c r="E42" s="80"/>
-      <c r="H42" s="93" t="s">
+      <c r="D42" s="69"/>
+      <c r="E42" s="70"/>
+      <c r="H42" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="I42" s="94"/>
+      <c r="I42" s="90"/>
     </row>
     <row r="43" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D43" s="79"/>
-      <c r="E43" s="80"/>
-      <c r="H43" s="74" t="s">
+      <c r="D43" s="69"/>
+      <c r="E43" s="70"/>
+      <c r="H43" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="I43" s="75"/>
+      <c r="I43" s="65"/>
     </row>
     <row r="44" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D44" s="79"/>
-      <c r="E44" s="80"/>
-      <c r="H44" s="89" t="s">
+      <c r="D44" s="69"/>
+      <c r="E44" s="70"/>
+      <c r="H44" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="I44" s="90"/>
+      <c r="I44" s="80"/>
     </row>
     <row r="45" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D45" s="81"/>
-      <c r="E45" s="82"/>
-      <c r="H45" s="91" t="s">
+      <c r="D45" s="71"/>
+      <c r="E45" s="72"/>
+      <c r="H45" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="I45" s="92"/>
+      <c r="I45" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="D8:E9"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="D39:E45"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H45:I45"/>
     <mergeCell ref="H19:I24"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="H42:I42"/>
@@ -2049,6 +2033,22 @@
     <mergeCell ref="F29:G29"/>
     <mergeCell ref="F19:G24"/>
     <mergeCell ref="D28:E28"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="D39:E45"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D8:E9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>